<commit_message>
Creating polynomial model and update dataset
</commit_message>
<xml_diff>
--- a/Sales.xlsx
+++ b/Sales.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\00-MLSamples\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yousif Ennwa\Documents\GitHub\Machine_Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F9BC6D-DB83-4E86-84AB-2A2AA79EB0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NewEmployees" sheetId="3" r:id="rId1"/>
-    <sheet name="Employees" sheetId="2" r:id="rId2"/>
-    <sheet name="Sales" sheetId="4" r:id="rId3"/>
+    <sheet name="Sales" sheetId="4" r:id="rId1"/>
+    <sheet name="NewEmployees" sheetId="3" r:id="rId2"/>
+    <sheet name="Employees" sheetId="2" r:id="rId3"/>
     <sheet name="ConcatenatedSheet" sheetId="1" r:id="rId4"/>
     <sheet name="Names" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -88,7 +99,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,6 +267,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -291,6 +319,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,7 +511,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1997</v>
+      </c>
+      <c r="B2" s="2">
+        <f>A2*0.25</f>
+        <v>499.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1998</v>
+      </c>
+      <c r="B3" s="2">
+        <f t="shared" ref="B3:B5" si="0">A3*0.25</f>
+        <v>499.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1999</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
+        <v>499.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2001</v>
+      </c>
+      <c r="B6" s="2">
+        <f>A6*0.5</f>
+        <v>1000.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2002</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" ref="B7:B10" si="1">A7*0.5</f>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2003</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="1"/>
+        <v>1001.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2004</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2005</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="1"/>
+        <v>1002.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2006</v>
+      </c>
+      <c r="B11" s="2">
+        <f>A11*0.75</f>
+        <v>1504.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2007</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" ref="B12:B15" si="2">A12*0.75</f>
+        <v>1505.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2008</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="2"/>
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>2009</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="2"/>
+        <v>1506.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2010</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="2"/>
+        <v>1507.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>2011</v>
+      </c>
+      <c r="B16" s="2">
+        <f>A16*1.5</f>
+        <v>3016.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2012</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" ref="B17:B21" si="3">A17*1.5</f>
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>2013</v>
+      </c>
+      <c r="B18" s="2">
+        <f t="shared" si="3"/>
+        <v>3019.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>2014</v>
+      </c>
+      <c r="B19" s="2">
+        <f t="shared" si="3"/>
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>2015</v>
+      </c>
+      <c r="B20" s="2">
+        <f t="shared" si="3"/>
+        <v>3022.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>2016</v>
+      </c>
+      <c r="B21" s="2">
+        <f t="shared" si="3"/>
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>2017</v>
+      </c>
+      <c r="B22" s="2">
+        <f>A22*3</f>
+        <v>6051</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>2018</v>
+      </c>
+      <c r="B23" s="2">
+        <f t="shared" ref="B23:B25" si="4">A23*3</f>
+        <v>6054</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>2019</v>
+      </c>
+      <c r="B24" s="2">
+        <f t="shared" si="4"/>
+        <v>6057</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -792,8 +1071,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1119,219 +1398,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1997</v>
-      </c>
-      <c r="B2" s="2">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1998</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1999</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>2000</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1277</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>2001</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>2002</v>
-      </c>
-      <c r="B7" s="2">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>2003</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1358</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>2004</v>
-      </c>
-      <c r="B9" s="2">
-        <v>1384</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>2005</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>2006</v>
-      </c>
-      <c r="B11" s="2">
-        <v>1436</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>2007</v>
-      </c>
-      <c r="B12" s="2">
-        <v>1462</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>2008</v>
-      </c>
-      <c r="B13" s="2">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>2009</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1514</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2010</v>
-      </c>
-      <c r="B15" s="2">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>2011</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1566</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>2012</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>2013</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1618</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>2014</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1644</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>2015</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1670</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>2016</v>
-      </c>
-      <c r="B21" s="2">
-        <v>1696</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>2017</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1722</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>2018</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1748</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>2019</v>
-      </c>
-      <c r="B24" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0"/>
@@ -1890,10 +1958,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>